<commit_message>
Add single-user JWT auth, login page, and bot protection
- JWT authentication via jose (Edge-compatible)
- Login page with dark theme matching app style
- Middleware gatekeeper: redirects unauthenticated users to /login
- Pages moved to (dashboard) route group with Sidebar layout
- Logout button in Sidebar footer
- robots.txt blocks all crawlers
- Security headers: X-Robots-Tag, X-Frame-Options, X-Content-Type-Options, Referrer-Policy
- robots meta tags in layout (noindex, nofollow)
- Utility scripts for DB management and scraper testing

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/products-template.xlsx
+++ b/products-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kenvue-my.sharepoint.com/personal/clinar01_kenvue_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisindanight/pharmacy-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="472" documentId="13_ncr:1_{A9B895EF-0157-8C4D-B883-E0FB4EB06A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C781311-591F-4720-9465-881C9F77381F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF52B37-C94C-7D4F-B903-7CFD7E8D46A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="23260" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL-uri Produse" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4635" uniqueCount="2098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="2097">
   <si>
     <t>Categorie</t>
   </si>
@@ -5103,9 +5103,6 @@
   </si>
   <si>
     <t>https://www.remediumfarm.ro/picaturi-pentru-nas/rhinxyl-ha-0-5mg-ml-spray-nazal-10ml-terapia</t>
-  </si>
-  <si>
-    <t>https://www.remediumfarm.ro/dureri-de-gat/faringosept-rapid-cu-gust-de-miere-si-lamaie-12-pastile-de-supt-terapia</t>
   </si>
   <si>
     <t>https://www.remediumfarm.ro/afectiuni-respiratorii/septosol-cu-albastru-de-metilen-20-comprimate-de-supt-biofarm</t>
@@ -6712,29 +6709,29 @@
   <dimension ref="A1:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.796875" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" customWidth="1"/>
-    <col min="4" max="4" width="7.796875" customWidth="1"/>
-    <col min="5" max="5" width="10.796875" customWidth="1"/>
-    <col min="6" max="6" width="8.19921875" customWidth="1"/>
-    <col min="7" max="7" width="11.296875" customWidth="1"/>
-    <col min="8" max="8" width="15.19921875" customWidth="1"/>
-    <col min="9" max="9" width="17.8984375" customWidth="1"/>
-    <col min="10" max="10" width="40.09765625" customWidth="1"/>
-    <col min="11" max="11" width="20.69921875" customWidth="1"/>
-    <col min="12" max="13" width="70.796875" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" customWidth="1"/>
+    <col min="10" max="10" width="40.1640625" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="13" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6775,7 +6772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -6816,7 +6813,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -6826,7 +6823,7 @@
       <c r="C3" s="4">
         <v>3574661839608</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -6842,22 +6839,22 @@
         <v>1663</v>
       </c>
       <c r="I3" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="K3" t="s">
         <v>1415</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -6883,22 +6880,22 @@
         <v>1664</v>
       </c>
       <c r="I4" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -6924,22 +6921,22 @@
         <v>1665</v>
       </c>
       <c r="I5" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="L5" t="s">
         <v>1415</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -6965,22 +6962,22 @@
         <v>1666</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="K6" t="s">
         <v>1415</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -7006,22 +7003,22 @@
         <v>1667</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="K7" t="s">
         <v>1415</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -7047,7 +7044,7 @@
         <v>1668</v>
       </c>
       <c r="I8" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="J8" t="s">
         <v>1415</v>
@@ -7056,13 +7053,13 @@
         <v>1415</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="M8" t="s">
         <v>1415</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -7088,13 +7085,13 @@
         <v>1669</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="L9" t="s">
         <v>1415</v>
@@ -7103,7 +7100,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -7141,10 +7138,10 @@
         <v>1415</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -7185,7 +7182,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -7226,7 +7223,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -7252,22 +7249,22 @@
         <v>1671</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="K13" t="s">
         <v>1415</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -7293,7 +7290,7 @@
         <v>1415</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="J14" t="s">
         <v>1415</v>
@@ -7305,10 +7302,10 @@
         <v>1415</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -7334,10 +7331,10 @@
         <v>1415</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="K15" t="s">
         <v>1415</v>
@@ -7346,10 +7343,10 @@
         <v>1415</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -7375,10 +7372,10 @@
         <v>1672</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="K16" t="s">
         <v>1415</v>
@@ -7387,10 +7384,10 @@
         <v>1415</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -7416,22 +7413,22 @@
         <v>1673</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="K17" t="s">
         <v>1415</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -7457,22 +7454,22 @@
         <v>1674</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -7498,22 +7495,22 @@
         <v>1675</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>2026</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -7539,22 +7536,22 @@
         <v>1676</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>2027</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -7580,22 +7577,22 @@
         <v>1677</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>2028</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -7633,10 +7630,10 @@
         <v>1415</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>2029</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -7662,22 +7659,22 @@
         <v>1678</v>
       </c>
       <c r="I23" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="K23" t="s">
         <v>1415</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -7703,22 +7700,22 @@
         <v>1679</v>
       </c>
       <c r="I24" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="K24" t="s">
         <v>1415</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>2031</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -7744,22 +7741,22 @@
         <v>1680</v>
       </c>
       <c r="I25" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="K25" t="s">
         <v>1415</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>2032</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -7785,22 +7782,22 @@
         <v>1415</v>
       </c>
       <c r="I26" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>2033</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -7826,22 +7823,22 @@
         <v>1681</v>
       </c>
       <c r="I27" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>2034</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -7867,22 +7864,22 @@
         <v>1682</v>
       </c>
       <c r="I28" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>2035</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -7908,22 +7905,22 @@
         <v>1683</v>
       </c>
       <c r="I29" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="K29" t="s">
         <v>1415</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>2036</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -7949,22 +7946,22 @@
         <v>1684</v>
       </c>
       <c r="I30" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>2037</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -7990,10 +7987,10 @@
         <v>1415</v>
       </c>
       <c r="I31" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="K31" t="s">
         <v>1415</v>
@@ -8002,10 +7999,10 @@
         <v>1415</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>2038</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -8031,22 +8028,22 @@
         <v>1685</v>
       </c>
       <c r="I32" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>2039</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -8072,10 +8069,10 @@
         <v>1686</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="K33" t="s">
         <v>1415</v>
@@ -8084,10 +8081,10 @@
         <v>1415</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -8113,22 +8110,22 @@
         <v>1687</v>
       </c>
       <c r="I34" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>2041</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -8154,22 +8151,22 @@
         <v>1415</v>
       </c>
       <c r="I35" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="L35" t="s">
         <v>1415</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>2042</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -8192,22 +8189,22 @@
         <v>1610</v>
       </c>
       <c r="I36" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>2043</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -8233,22 +8230,22 @@
         <v>1688</v>
       </c>
       <c r="I37" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K37" t="s">
         <v>1415</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>2044</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -8274,22 +8271,22 @@
         <v>1689</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="K38" t="s">
         <v>1415</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -8330,7 +8327,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -8371,7 +8368,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -8397,22 +8394,22 @@
         <v>1690</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="K41" t="s">
         <v>1415</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>2046</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -8438,22 +8435,22 @@
         <v>1691</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="K42" t="s">
         <v>1415</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>2047</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -8479,22 +8476,22 @@
         <v>1692</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -8520,22 +8517,22 @@
         <v>1693</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>2049</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>145</v>
       </c>
@@ -8558,25 +8555,25 @@
         <v>1617</v>
       </c>
       <c r="H45" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="K45" t="s">
         <v>1415</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>145</v>
       </c>
@@ -8598,26 +8595,26 @@
       <c r="G46" t="s">
         <v>1618</v>
       </c>
-      <c r="H46" t="s">
-        <v>1694</v>
+      <c r="H46" s="1" t="s">
+        <v>1415</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="K46" t="s">
         <v>1415</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>2051</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>145</v>
       </c>
@@ -8625,9 +8622,9 @@
         <v>152</v>
       </c>
       <c r="C47" s="4">
-        <v>8000036013076</v>
-      </c>
-      <c r="D47" t="s">
+        <v>5944702001871</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -8640,25 +8637,25 @@
         <v>1620</v>
       </c>
       <c r="H47" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>2052</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>145</v>
       </c>
@@ -8684,22 +8681,22 @@
         <v>1415</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="K48" t="s">
         <v>1415</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>2053</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -8722,25 +8719,25 @@
         <v>1621</v>
       </c>
       <c r="H49" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="K49" t="s">
         <v>1415</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>2054</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>145</v>
       </c>
@@ -8763,25 +8760,25 @@
         <v>1415</v>
       </c>
       <c r="H50" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="K50" t="s">
         <v>1415</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>145</v>
       </c>
@@ -8804,25 +8801,25 @@
         <v>1622</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>2056</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>145</v>
       </c>
@@ -8845,25 +8842,25 @@
         <v>1623</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>2057</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>145</v>
       </c>
@@ -8886,25 +8883,25 @@
         <v>1624</v>
       </c>
       <c r="H53" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>2058</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>145</v>
       </c>
@@ -8927,10 +8924,10 @@
         <v>1625</v>
       </c>
       <c r="H54" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="J54" t="s">
         <v>1415</v>
@@ -8942,10 +8939,10 @@
         <v>1415</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>2059</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>145</v>
       </c>
@@ -8968,25 +8965,25 @@
         <v>1626</v>
       </c>
       <c r="H55" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>2060</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>145</v>
       </c>
@@ -9009,25 +9006,25 @@
         <v>1627</v>
       </c>
       <c r="H56" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>2061</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>145</v>
       </c>
@@ -9050,25 +9047,25 @@
         <v>1628</v>
       </c>
       <c r="H57" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>2062</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>145</v>
       </c>
@@ -9091,25 +9088,25 @@
         <v>1629</v>
       </c>
       <c r="H58" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>2063</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>188</v>
       </c>
@@ -9132,25 +9129,25 @@
         <v>1630</v>
       </c>
       <c r="H59" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>2064</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>188</v>
       </c>
@@ -9173,25 +9170,25 @@
         <v>1631</v>
       </c>
       <c r="H60" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>2065</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>188</v>
       </c>
@@ -9214,13 +9211,13 @@
         <v>1632</v>
       </c>
       <c r="H61" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="K61" t="s">
         <v>1415</v>
@@ -9229,10 +9226,10 @@
         <v>1415</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>2066</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>188</v>
       </c>
@@ -9255,25 +9252,25 @@
         <v>1633</v>
       </c>
       <c r="H62" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K62" t="s">
         <v>1415</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>2067</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>201</v>
       </c>
@@ -9296,25 +9293,25 @@
         <v>1634</v>
       </c>
       <c r="H63" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>2068</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>201</v>
       </c>
@@ -9337,25 +9334,25 @@
         <v>1635</v>
       </c>
       <c r="H64" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>2069</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>201</v>
       </c>
@@ -9378,25 +9375,25 @@
         <v>1636</v>
       </c>
       <c r="H65" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>201</v>
       </c>
@@ -9419,25 +9416,25 @@
         <v>1637</v>
       </c>
       <c r="H66" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="J66" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>2072</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>201</v>
       </c>
@@ -9460,25 +9457,25 @@
         <v>1638</v>
       </c>
       <c r="H67" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>2071</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>201</v>
       </c>
@@ -9501,25 +9498,25 @@
         <v>1639</v>
       </c>
       <c r="H68" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="K68" t="s">
         <v>1415</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>2073</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -9542,25 +9539,25 @@
         <v>1640</v>
       </c>
       <c r="H69" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="K69" t="s">
         <v>1415</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>2074</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -9583,25 +9580,25 @@
         <v>1641</v>
       </c>
       <c r="H70" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="K70" t="s">
         <v>1415</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>2075</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>201</v>
       </c>
@@ -9624,25 +9621,25 @@
         <v>1642</v>
       </c>
       <c r="H71" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="K71" t="s">
         <v>1415</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>2076</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>201</v>
       </c>
@@ -9665,25 +9662,25 @@
         <v>1415</v>
       </c>
       <c r="H72" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="K72" t="s">
         <v>1415</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>2077</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>201</v>
       </c>
@@ -9709,22 +9706,22 @@
         <v>1415</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="K73" t="s">
         <v>1415</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>2078</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>201</v>
       </c>
@@ -9747,25 +9744,25 @@
         <v>1644</v>
       </c>
       <c r="H74" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>2079</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>201</v>
       </c>
@@ -9788,25 +9785,25 @@
         <v>1645</v>
       </c>
       <c r="H75" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>2080</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>201</v>
       </c>
@@ -9829,25 +9826,25 @@
         <v>1646</v>
       </c>
       <c r="H76" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>2081</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -9870,25 +9867,25 @@
         <v>1647</v>
       </c>
       <c r="H77" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="K77" t="s">
         <v>1415</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>2082</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>201</v>
       </c>
@@ -9911,25 +9908,25 @@
         <v>1648</v>
       </c>
       <c r="H78" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="K78" t="s">
         <v>1415</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>2083</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>250</v>
       </c>
@@ -9952,25 +9949,25 @@
         <v>1649</v>
       </c>
       <c r="H79" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>2084</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>250</v>
       </c>
@@ -9993,25 +9990,25 @@
         <v>1650</v>
       </c>
       <c r="H80" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>2085</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>250</v>
       </c>
@@ -10034,25 +10031,25 @@
         <v>1651</v>
       </c>
       <c r="H81" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="L81" t="s">
         <v>1415</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>2086</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>250</v>
       </c>
@@ -10078,10 +10075,10 @@
         <v>1415</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="K82" t="s">
         <v>1415</v>
@@ -10090,10 +10087,10 @@
         <v>1415</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>2087</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>250</v>
       </c>
@@ -10116,25 +10113,25 @@
         <v>1653</v>
       </c>
       <c r="H83" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="L83" t="s">
         <v>1415</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>2088</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>250</v>
       </c>
@@ -10157,25 +10154,25 @@
         <v>1654</v>
       </c>
       <c r="H84" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="L84" t="s">
         <v>1415</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>2089</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>250</v>
       </c>
@@ -10198,25 +10195,25 @@
         <v>1655</v>
       </c>
       <c r="H85" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="L85" t="s">
         <v>1415</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>250</v>
       </c>
@@ -10239,25 +10236,25 @@
         <v>1656</v>
       </c>
       <c r="H86" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>2091</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>275</v>
       </c>
@@ -10280,25 +10277,25 @@
         <v>1657</v>
       </c>
       <c r="H87" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="L87" t="s">
         <v>1415</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>2092</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>275</v>
       </c>
@@ -10324,22 +10321,22 @@
         <v>1415</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="K88" t="s">
         <v>1415</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>2093</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>275</v>
       </c>
@@ -10362,25 +10359,25 @@
         <v>1659</v>
       </c>
       <c r="H89" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="L89" t="s">
         <v>1415</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>2094</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>275</v>
       </c>
@@ -10403,25 +10400,25 @@
         <v>1660</v>
       </c>
       <c r="H90" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="K90" t="s">
         <v>1415</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>2095</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>290</v>
       </c>
@@ -10434,7 +10431,7 @@
       <c r="D91" s="1" t="s">
         <v>1581</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="1" t="s">
         <v>293</v>
       </c>
       <c r="F91" s="1" t="s">
@@ -10444,25 +10441,25 @@
         <v>1661</v>
       </c>
       <c r="H91" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>2096</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>290</v>
       </c>
@@ -10472,7 +10469,7 @@
       <c r="C92" s="4">
         <v>4013054025185</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="1" t="s">
         <v>1583</v>
       </c>
       <c r="E92" t="s">
@@ -10485,22 +10482,22 @@
         <v>1662</v>
       </c>
       <c r="H92" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
     </row>
   </sheetData>
@@ -11028,10 +11025,15 @@
     <hyperlink ref="M90" r:id="rId521" xr:uid="{07B3CD7F-6F69-42A0-B337-B06D744E62B7}"/>
     <hyperlink ref="M91" r:id="rId522" xr:uid="{17E2066D-738D-4248-AF83-999DB433F767}"/>
     <hyperlink ref="M92" r:id="rId523" xr:uid="{89EFF58F-1B19-4E0C-9C8E-F4234C7A335D}"/>
+    <hyperlink ref="E91" r:id="rId524" xr:uid="{A843AF66-9D8E-4045-B037-B281AEF36E05}"/>
+    <hyperlink ref="D3" r:id="rId525" xr:uid="{25F05B1F-0802-6545-BF9B-3DC2FD24D2A3}"/>
+    <hyperlink ref="D47" r:id="rId526" xr:uid="{BBD40ED4-952E-E540-BBDA-478714409033}"/>
+    <hyperlink ref="D92" r:id="rId527" xr:uid="{FF38291E-223F-9A4A-996E-15FA94CE97B0}"/>
+    <hyperlink ref="H46" r:id="rId528" display="https://www.remediumfarm.ro/dureri-de-gat/faringosept-rapid-cu-gust-de-miere-si-lamaie-12-pastile-de-supt-terapia" xr:uid="{6ADF4E4D-0709-FF4A-A998-91EAF1F78C98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H1 A15:D15 A2:D2 A3:B3 A4:D4 A5:B5 A6:D6 A7:D7 A8:D8 A9:D9 A10:D10 A11 C11:D11 A12:D12 A35:D35 A16:B16 D16 A17:D17 A18:B18 D18 A19:D19 A20:D20 A21:D21 A22:D22 A23:D23 A24:D24 A25:D25 A26:B26 D26 A27:D27 A28:D28 A29:D29 A30 A31:D31 A32:D32 A90:C90 A36:D36 A33:D33 A34:D34 A13:D13 A14:D14 A37:D37 A38:D38 A39:B39 A40:D40 A41:B41 A42:B42 A43:D43 A44:B44 A45:B45 A46:B46 A47:B47 A48:B48 A49:B49 A50:B50 A51:B51 D51 A52:B52 D52 A53 A54:B54 A55:D55 A56 A57:D57 A58:B58 A59:D59 A60:B60 A61 A62 A63:B63 A64:D64 A65 A66:B66 A67:D67 A68:D68 A69:B69 A70:B70 A71:D71 A72:D72 A73:D73 A74 A75:D75 A76:D76 A77:D77 A78:D78 A79:D79 A80:B80 A81:D81 A82:D82 A83 A84:D84 A85:D85 A86 A87:D87 D30 A92:B92 A91:B91 D56 C83:D83 A88:C88 A89:C89 E91 E92 E90 E89 E88 I1:K1 I12 L1:M1 D45 D47 D39 D41 D42 D44 D46 D48 D49 D50 D53 D54 D58 D60 D61 D63 D65 D66 D69 D70 D80 D86 D5 C62:D62 D3 C74:D74" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 A15:D15 A2:D2 A3 A4:D4 A5:B5 A6:D6 A7:D7 A8:D8 A9:D9 A10:D10 A11 C11:D11 A12:D12 A35:D35 A16:B16 D16 A17:D17 A18:B18 D18 A19:D19 A20:D20 A21:D21 A22:D22 A23:D23 A24:D24 A25:D25 A26:B26 D26 A27:D27 A28:D28 A29:D29 A30 A31:D31 A32:D32 A90:C90 A36:D36 A33:D33 A34:D34 A13:D13 A14:D14 A37:D37 A38:D38 A39:B39 A40:D40 A41:B41 A42:B42 A43:D43 A44:B44 A45:B45 A46:B46 A47:B47 A48:B48 A49:B49 A50:B50 A51:B51 D51 A52:B52 D52 A53 A54:B54 A55:D55 A56 A57:D57 A58:B58 A59:D59 A60:B60 A61 A62 A63:B63 A64:D64 A65 A66:B66 A67:D67 A68:D68 A69:B69 A70:B70 A71:D71 A72:D72 A73:D73 A74 A75:D75 A76:D76 A77:D77 A78:D78 A79:D79 A80:B80 A81:D81 A82:D82 A83 A84:D84 A85:D85 A86 A87:D87 D30 A92:B92 A91:B91 D56 C83:D83 A88:C88 A89:C89 E92 E90 E89 E88 I1:K1 I12 L1:M1 D45 D39 D41 D42 D44 D46 D48 D49 D50 D53 D54 D58 D60 D61 D63 D65 D66 D69 D70 D80 D86 D5 C62:D62 C74:D74" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -11044,14 +11046,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.796875" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" customWidth="1"/>
-    <col min="3" max="14" width="80.796875" customWidth="1"/>
+    <col min="1" max="1" width="45.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="14" width="80.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -11095,7 +11097,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -11139,7 +11141,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -11183,7 +11185,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -11227,7 +11229,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -11271,7 +11273,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -11315,7 +11317,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -11359,7 +11361,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -11403,7 +11405,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -11447,7 +11449,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -11491,7 +11493,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -11535,7 +11537,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -11579,7 +11581,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -11623,7 +11625,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -11667,7 +11669,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -11711,7 +11713,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -11755,7 +11757,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -11799,7 +11801,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -11843,7 +11845,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -11887,7 +11889,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -11931,7 +11933,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -11975,7 +11977,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -12019,7 +12021,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -12063,7 +12065,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -12107,7 +12109,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -12151,7 +12153,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -12195,7 +12197,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -12239,7 +12241,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -12283,7 +12285,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -12327,7 +12329,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -12371,7 +12373,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -12415,7 +12417,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -12459,7 +12461,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>109</v>
       </c>
@@ -12503,7 +12505,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>112</v>
       </c>
@@ -12547,7 +12549,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>115</v>
       </c>
@@ -12591,7 +12593,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -12635,7 +12637,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -12679,7 +12681,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>124</v>
       </c>
@@ -12723,7 +12725,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>127</v>
       </c>
@@ -12767,7 +12769,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>130</v>
       </c>
@@ -12811,7 +12813,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -12855,7 +12857,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>136</v>
       </c>
@@ -12899,7 +12901,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -12943,7 +12945,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>142</v>
       </c>
@@ -12987,7 +12989,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>146</v>
       </c>
@@ -13031,7 +13033,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>149</v>
       </c>
@@ -13075,7 +13077,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>152</v>
       </c>
@@ -13119,7 +13121,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>155</v>
       </c>
@@ -13163,7 +13165,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>158</v>
       </c>
@@ -13207,7 +13209,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>161</v>
       </c>
@@ -13251,7 +13253,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>164</v>
       </c>
@@ -13295,7 +13297,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>167</v>
       </c>
@@ -13339,7 +13341,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -13383,7 +13385,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>173</v>
       </c>
@@ -13427,7 +13429,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>176</v>
       </c>
@@ -13471,7 +13473,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -13515,7 +13517,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>182</v>
       </c>
@@ -13559,7 +13561,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>185</v>
       </c>
@@ -13603,7 +13605,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>189</v>
       </c>
@@ -13647,7 +13649,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>192</v>
       </c>
@@ -13691,7 +13693,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>195</v>
       </c>
@@ -13735,7 +13737,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>198</v>
       </c>
@@ -13779,7 +13781,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>202</v>
       </c>
@@ -13823,7 +13825,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>205</v>
       </c>
@@ -13867,7 +13869,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>208</v>
       </c>
@@ -13911,7 +13913,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>211</v>
       </c>
@@ -13955,7 +13957,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>214</v>
       </c>
@@ -13999,7 +14001,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>217</v>
       </c>
@@ -14043,7 +14045,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>220</v>
       </c>
@@ -14087,7 +14089,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>223</v>
       </c>
@@ -14131,7 +14133,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>226</v>
       </c>
@@ -14175,7 +14177,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>229</v>
       </c>
@@ -14219,7 +14221,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>232</v>
       </c>
@@ -14263,7 +14265,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>235</v>
       </c>
@@ -14307,7 +14309,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>238</v>
       </c>
@@ -14351,7 +14353,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>241</v>
       </c>
@@ -14395,7 +14397,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>244</v>
       </c>
@@ -14439,7 +14441,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>247</v>
       </c>
@@ -14483,7 +14485,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>251</v>
       </c>
@@ -14527,7 +14529,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>254</v>
       </c>
@@ -14571,7 +14573,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>257</v>
       </c>
@@ -14615,7 +14617,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>260</v>
       </c>
@@ -14659,7 +14661,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>263</v>
       </c>
@@ -14703,7 +14705,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>266</v>
       </c>
@@ -14747,7 +14749,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>269</v>
       </c>
@@ -14791,7 +14793,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>272</v>
       </c>
@@ -14835,7 +14837,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>276</v>
       </c>
@@ -14879,7 +14881,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>279</v>
       </c>
@@ -14923,7 +14925,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>281</v>
       </c>
@@ -14967,7 +14969,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>284</v>
       </c>
@@ -15011,7 +15013,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>287</v>
       </c>
@@ -15055,7 +15057,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>291</v>
       </c>
@@ -15099,7 +15101,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>294</v>
       </c>

</xml_diff>